<commit_message>
Improve Excel report formatting for auditor readability and data structure
Update `writer_agent.py` to enhance the Excel report generation by applying professional styling, adjusting column widths for better readability, and ensuring data is structured for auditor use. This includes cleaning shop names and mapping data to specific columns with appropriate formatting.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 85863112-a031-405a-83ae-302c869661f0
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/a76d741b-8ad6-464e-a09a-fc6953be1e99/85863112-a031-405a-83ae-302c869661f0/38r4T5N
</commit_message>
<xml_diff>
--- a/python_backend/output/Sample_GST_Extract.xlsx
+++ b/python_backend/output/Sample_GST_Extract.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="GST Report" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="GST Audit Report" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -26,18 +26,45 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Arial"/>
       <b val="1"/>
+      <color rgb="00FFFFFF"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <b val="1"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <i val="1"/>
+      <sz val="9"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="9"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="002B5D84"/>
+        <bgColor rgb="002B5D84"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -45,16 +72,68 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -420,138 +499,194 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="18" customWidth="1" min="1" max="1"/>
-    <col width="18" customWidth="1" min="2" max="2"/>
+    <col width="8" customWidth="1" min="1" max="1"/>
+    <col width="25" customWidth="1" min="2" max="2"/>
     <col width="18" customWidth="1" min="3" max="3"/>
-    <col width="18" customWidth="1" min="4" max="4"/>
-    <col width="18" customWidth="1" min="5" max="5"/>
-    <col width="18" customWidth="1" min="6" max="6"/>
-    <col width="18" customWidth="1" min="7" max="7"/>
-    <col width="18" customWidth="1" min="8" max="8"/>
-    <col width="18" customWidth="1" min="9" max="9"/>
-    <col width="30" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
+    <col width="12" customWidth="1" min="8" max="8"/>
+    <col width="12" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="10" max="10"/>
+    <col width="35" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="30" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Shop Name</t>
+          <t>S.No.</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Vendor/Shop Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>GSTIN</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Invoice Number</t>
-        </is>
-      </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Invoice Date</t>
+          <t>Invoice No.</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Total Amount</t>
+          <t>Date</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Tax Amount</t>
+          <t>Taxable Amount</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>Total Tax</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>CGST</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>SGST</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>IGST</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>HSN Code</t>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>HSN Codes</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>WESTSIDE
-Sjr Zion, Survey</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
+    <row r="2" ht="25" customHeight="1">
+      <c r="A2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>WESTSIDE, Sjr Zion, Survey</t>
+        </is>
+      </c>
+      <c r="C2" s="4" t="inlineStr">
         <is>
           <t>29AAACL1838J1ZC</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" s="4" t="inlineStr">
         <is>
           <t>W089 100169940</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" s="4" t="inlineStr">
         <is>
           <t>2024-09-28</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" s="4" t="inlineStr">
         <is>
           <t>4045.01</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" s="4" t="inlineStr">
         <is>
           <t>173.91</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" s="4" t="inlineStr">
         <is>
           <t>173.91</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" s="4" t="inlineStr">
         <is>
           <t>173.91</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" s="4" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="J2" s="2" t="inlineStr">
-        <is>
-          <t>996211
-62052000
-62052000
-62046200
-48194000
-33072000
-39264099</t>
+      <c r="K2" s="3" t="inlineStr">
+        <is>
+          <t>996211, 62052000, 62052000, 62046200, 48194000, 33072000, 39264099</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+      <c r="B3" s="6" t="n"/>
+      <c r="C3" s="6" t="n"/>
+      <c r="D3" s="6" t="n"/>
+      <c r="E3" s="7" t="n"/>
+      <c r="F3" s="8" t="inlineStr">
+        <is>
+          <t>₹4,045.01</t>
+        </is>
+      </c>
+      <c r="G3" s="8" t="inlineStr">
+        <is>
+          <t>₹173.91</t>
+        </is>
+      </c>
+      <c r="H3" s="8" t="inlineStr">
+        <is>
+          <t>₹173.91</t>
+        </is>
+      </c>
+      <c r="I3" s="8" t="inlineStr">
+        <is>
+          <t>₹173.91</t>
+        </is>
+      </c>
+      <c r="J3" s="8" t="inlineStr">
+        <is>
+          <t>₹0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="9" t="inlineStr">
+        <is>
+          <t>Generated for GST Audit Purposes</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="10" t="inlineStr">
+        <is>
+          <t>Total Invoices: 1</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A3:E3"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>